<commit_message>
Initial analysis on QST and CST
</commit_message>
<xml_diff>
--- a/data/RAW-DATA.xlsx
+++ b/data/RAW-DATA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="QST &amp; CST Analysis" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Customer ID</t>
   </si>
@@ -65,12 +65,33 @@
   <si>
     <t>Max</t>
   </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Histogram Output</t>
+  </si>
+  <si>
+    <t>Bin Ranges</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>General Statistics</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,6 +107,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -95,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -103,11 +148,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -119,8 +214,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="3" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -134,6 +262,650 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Queue Service</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Time (QZ)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'QST &amp; CST Analysis'!$L$4:$L$34</c:f>
+              <c:strCache>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>More</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'QST &amp; CST Analysis'!$M$4:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="418074192"/>
+        <c:axId val="418074584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="418074192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="418074584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="418074584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="418074192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cashier Service Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'QST &amp; CST Analysis'!$N$4:$N$14</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>More</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'QST &amp; CST Analysis'!$O$4:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="566528616"/>
+        <c:axId val="566527832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="566528616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="566527832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="566527832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="566528616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1787,37 +2559,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.75" style="4" customWidth="1"/>
     <col min="2" max="2" width="5.375" style="4" customWidth="1"/>
     <col min="3" max="3" width="6.375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="8" max="8" width="9" style="5"/>
+    <col min="9" max="9" width="9.75" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="I1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="L1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1827,74 +2614,148 @@
       <c r="C2" s="1">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="11"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="F3" s="14">
         <f>AVERAGE(B2:B61)</f>
         <v>97.783333333333331</v>
       </c>
-      <c r="G2">
+      <c r="G3" s="14">
         <f>AVERAGE(C2:C61)</f>
         <v>15.35</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>63</v>
-      </c>
-      <c r="C3" s="1">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>81</v>
+      </c>
+      <c r="C4" s="1">
+        <v>13</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F3">
+      <c r="F4" s="1">
         <f>MIN(B2:B61)</f>
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="G4" s="1">
         <f>MIN(C2:C61)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>81</v>
-      </c>
-      <c r="C4" s="1">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="I4" s="1">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
+        <v>5</v>
+      </c>
+      <c r="L4" s="6">
+        <v>10</v>
+      </c>
+      <c r="M4" s="7">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6">
+        <v>5</v>
+      </c>
+      <c r="O4" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>99</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F4">
+      <c r="F5" s="1">
         <f>MAX(B2:B61)</f>
         <v>497</v>
       </c>
-      <c r="G4">
+      <c r="G5" s="1">
         <f>MAX(C2:C61)</f>
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>99</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="1">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1">
+        <v>10</v>
+      </c>
+      <c r="L5" s="6">
+        <v>20</v>
+      </c>
+      <c r="M5" s="7">
+        <v>2</v>
+      </c>
+      <c r="N5" s="6">
+        <v>10</v>
+      </c>
+      <c r="O5" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1904,8 +2765,26 @@
       <c r="C6" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="1">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1">
+        <v>15</v>
+      </c>
+      <c r="L6" s="6">
+        <v>30</v>
+      </c>
+      <c r="M6" s="7">
+        <v>6</v>
+      </c>
+      <c r="N6" s="6">
+        <v>15</v>
+      </c>
+      <c r="O6" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1915,8 +2794,26 @@
       <c r="C7" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="1">
+        <v>40</v>
+      </c>
+      <c r="J7" s="1">
+        <v>20</v>
+      </c>
+      <c r="L7" s="6">
+        <v>40</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <v>20</v>
+      </c>
+      <c r="O7" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1926,8 +2823,26 @@
       <c r="C8" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>50</v>
+      </c>
+      <c r="J8" s="1">
+        <v>25</v>
+      </c>
+      <c r="L8" s="6">
+        <v>50</v>
+      </c>
+      <c r="M8" s="7">
+        <v>6</v>
+      </c>
+      <c r="N8" s="6">
+        <v>25</v>
+      </c>
+      <c r="O8" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1937,8 +2852,26 @@
       <c r="C9" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <v>60</v>
+      </c>
+      <c r="J9" s="1">
+        <v>30</v>
+      </c>
+      <c r="L9" s="6">
+        <v>60</v>
+      </c>
+      <c r="M9" s="7">
+        <v>7</v>
+      </c>
+      <c r="N9" s="6">
+        <v>30</v>
+      </c>
+      <c r="O9" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1948,8 +2881,26 @@
       <c r="C10" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>70</v>
+      </c>
+      <c r="J10" s="1">
+        <v>35</v>
+      </c>
+      <c r="L10" s="6">
+        <v>70</v>
+      </c>
+      <c r="M10" s="7">
+        <v>2</v>
+      </c>
+      <c r="N10" s="6">
+        <v>35</v>
+      </c>
+      <c r="O10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1959,8 +2910,26 @@
       <c r="C11" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <v>80</v>
+      </c>
+      <c r="J11" s="1">
+        <v>40</v>
+      </c>
+      <c r="L11" s="6">
+        <v>80</v>
+      </c>
+      <c r="M11" s="7">
+        <v>3</v>
+      </c>
+      <c r="N11" s="6">
+        <v>40</v>
+      </c>
+      <c r="O11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1970,8 +2939,26 @@
       <c r="C12" s="1">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <v>90</v>
+      </c>
+      <c r="J12" s="1">
+        <v>45</v>
+      </c>
+      <c r="L12" s="6">
+        <v>90</v>
+      </c>
+      <c r="M12" s="7">
+        <v>2</v>
+      </c>
+      <c r="N12" s="6">
+        <v>45</v>
+      </c>
+      <c r="O12" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1981,8 +2968,26 @@
       <c r="C13" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="1">
+        <v>100</v>
+      </c>
+      <c r="J13" s="1">
+        <v>50</v>
+      </c>
+      <c r="L13" s="6">
+        <v>100</v>
+      </c>
+      <c r="M13" s="7">
+        <v>4</v>
+      </c>
+      <c r="N13" s="6">
+        <v>50</v>
+      </c>
+      <c r="O13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1992,8 +2997,24 @@
       <c r="C14" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="1">
+        <v>110</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="L14" s="6">
+        <v>110</v>
+      </c>
+      <c r="M14" s="7">
+        <v>4</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2003,8 +3024,20 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="1">
+        <v>120</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="L15" s="6">
+        <v>120</v>
+      </c>
+      <c r="M15" s="7">
+        <v>6</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2014,8 +3047,20 @@
       <c r="C16" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I16" s="1">
+        <v>130</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="L16" s="6">
+        <v>130</v>
+      </c>
+      <c r="M16" s="7">
+        <v>1</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2025,8 +3070,20 @@
       <c r="C17" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <v>140</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="L17" s="6">
+        <v>140</v>
+      </c>
+      <c r="M17" s="7">
+        <v>2</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2036,8 +3093,20 @@
       <c r="C18" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I18" s="1">
+        <v>150</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="L18" s="6">
+        <v>150</v>
+      </c>
+      <c r="M18" s="7">
+        <v>3</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="7"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2047,8 +3116,20 @@
       <c r="C19" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <v>160</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="L19" s="6">
+        <v>160</v>
+      </c>
+      <c r="M19" s="7">
+        <v>3</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2058,8 +3139,18 @@
       <c r="C20" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I20" s="1">
+        <v>170</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="L20" s="6">
+        <v>170</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2069,8 +3160,18 @@
       <c r="C21" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I21" s="1">
+        <v>180</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="L21" s="6">
+        <v>180</v>
+      </c>
+      <c r="M21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2080,8 +3181,18 @@
       <c r="C22" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I22" s="1">
+        <v>190</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="L22" s="6">
+        <v>190</v>
+      </c>
+      <c r="M22" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2091,8 +3202,18 @@
       <c r="C23" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I23" s="1">
+        <v>200</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="L23" s="6">
+        <v>200</v>
+      </c>
+      <c r="M23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2102,8 +3223,18 @@
       <c r="C24" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I24" s="1">
+        <v>210</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="L24" s="6">
+        <v>210</v>
+      </c>
+      <c r="M24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2113,8 +3244,18 @@
       <c r="C25" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I25" s="1">
+        <v>220</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="L25" s="6">
+        <v>220</v>
+      </c>
+      <c r="M25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2124,8 +3265,18 @@
       <c r="C26" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I26" s="1">
+        <v>230</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="L26" s="6">
+        <v>230</v>
+      </c>
+      <c r="M26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2135,8 +3286,18 @@
       <c r="C27" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I27" s="1">
+        <v>240</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="L27" s="6">
+        <v>240</v>
+      </c>
+      <c r="M27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2146,8 +3307,18 @@
       <c r="C28" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I28" s="1">
+        <v>250</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="L28" s="6">
+        <v>250</v>
+      </c>
+      <c r="M28" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2157,8 +3328,18 @@
       <c r="C29" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I29" s="1">
+        <v>260</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="L29" s="6">
+        <v>260</v>
+      </c>
+      <c r="M29" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2168,8 +3349,18 @@
       <c r="C30" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I30" s="1">
+        <v>270</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="L30" s="6">
+        <v>270</v>
+      </c>
+      <c r="M30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2179,8 +3370,18 @@
       <c r="C31" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I31" s="1">
+        <v>280</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="L31" s="6">
+        <v>280</v>
+      </c>
+      <c r="M31" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2190,8 +3391,18 @@
       <c r="C32" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I32" s="1">
+        <v>290</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="L32" s="6">
+        <v>290</v>
+      </c>
+      <c r="M32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2201,8 +3412,18 @@
       <c r="C33" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I33" s="1">
+        <v>300</v>
+      </c>
+      <c r="J33" s="1"/>
+      <c r="L33" s="6">
+        <v>300</v>
+      </c>
+      <c r="M33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2212,8 +3433,14 @@
       <c r="C34" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L34" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M34" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2223,8 +3450,10 @@
       <c r="C35" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L35" s="6"/>
+      <c r="M35" s="7"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2234,8 +3463,10 @@
       <c r="C36" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L36" s="6"/>
+      <c r="M36" s="7"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2245,8 +3476,10 @@
       <c r="C37" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L37" s="6"/>
+      <c r="M37" s="7"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2256,8 +3489,10 @@
       <c r="C38" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L38" s="6"/>
+      <c r="M38" s="7"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2267,8 +3502,10 @@
       <c r="C39" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L39" s="6"/>
+      <c r="M39" s="7"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2278,8 +3515,10 @@
       <c r="C40" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L40" s="6"/>
+      <c r="M40" s="7"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2289,8 +3528,10 @@
       <c r="C41" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L41" s="6"/>
+      <c r="M41" s="7"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2300,8 +3541,10 @@
       <c r="C42" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L42" s="6"/>
+      <c r="M42" s="7"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2311,8 +3554,10 @@
       <c r="C43" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L43" s="6"/>
+      <c r="M43" s="7"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2322,8 +3567,10 @@
       <c r="C44" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L44" s="6"/>
+      <c r="M44" s="7"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2333,8 +3580,10 @@
       <c r="C45" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L45" s="6"/>
+      <c r="M45" s="7"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2344,8 +3593,10 @@
       <c r="C46" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L46" s="6"/>
+      <c r="M46" s="7"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2355,8 +3606,10 @@
       <c r="C47" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L47" s="6"/>
+      <c r="M47" s="7"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2366,8 +3619,10 @@
       <c r="C48" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L48" s="6"/>
+      <c r="M48" s="7"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2377,8 +3632,10 @@
       <c r="C49" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L49" s="6"/>
+      <c r="M49" s="7"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2388,8 +3645,10 @@
       <c r="C50" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L50" s="6"/>
+      <c r="M50" s="7"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2399,8 +3658,10 @@
       <c r="C51" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L51" s="6"/>
+      <c r="M51" s="7"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2410,8 +3671,10 @@
       <c r="C52" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L52" s="6"/>
+      <c r="M52" s="7"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2421,8 +3684,10 @@
       <c r="C53" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L53" s="6"/>
+      <c r="M53" s="7"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2433,7 +3698,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2444,7 +3709,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2455,7 +3720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2466,7 +3731,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2477,7 +3742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2488,7 +3753,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2499,7 +3764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2511,7 +3776,21 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="N4:N13">
+    <sortCondition ref="N4"/>
+  </sortState>
+  <mergeCells count="8">
+    <mergeCell ref="H1:H1048576"/>
+    <mergeCell ref="D1:D1048576"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="K1:K1048576"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Arrival Rate Histograms
</commit_message>
<xml_diff>
--- a/data/RAW-DATA.xlsx
+++ b/data/RAW-DATA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>Customer ID</t>
   </si>
@@ -99,6 +99,33 @@
   <si>
     <t># Customers</t>
   </si>
+  <si>
+    <t>1 Min</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>10min</t>
+  </si>
+  <si>
+    <t>Avg rate / 10min</t>
+  </si>
+  <si>
+    <t>Avg rate / 5 min</t>
+  </si>
+  <si>
+    <t>Avg rate / 1 min</t>
+  </si>
+  <si>
+    <t>1 min Interval</t>
+  </si>
+  <si>
+    <t>5 min Interval</t>
+  </si>
 </sst>
 </file>
 
@@ -153,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -208,6 +235,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -215,7 +253,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -257,6 +295,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -265,6 +306,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -287,6 +337,975 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>1 Minute Interval</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Arrival Rate Analysis'!$J$4:$J$64</c:f>
+              <c:strCache>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1020</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1140</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1260</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1620</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1740</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1860</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2160</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2220</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2280</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2340</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2460</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2520</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2580</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2640</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2760</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2820</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2880</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2940</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3060</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3120</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3180</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3240</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3360</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3420</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3480</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3540</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>More</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arrival Rate Analysis'!$K$4:$K$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="61"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="344619600"/>
+        <c:axId val="344620776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="344619600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="344620776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="344620776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="344619600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>5 Minute Interval</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Arrival Rate Analysis'!$L$4:$L$16</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>More</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arrival Rate Analysis'!$M$4:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="382856368"/>
+        <c:axId val="388272256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="382856368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="388272256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="388272256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="382856368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>10 Minute Interval</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Arrival Rate Analysis'!$N$4:$N$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>More</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Arrival Rate Analysis'!$O$4:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="388270688"/>
+        <c:axId val="386197928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="388270688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="386197928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="386197928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="388270688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -638,7 +1657,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -866,6 +1885,101 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1275,26 +2389,26 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="L2" s="18" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="L2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="Q2" s="18" t="s">
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="Q2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="18"/>
+      <c r="R2" s="19"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3620,1071 +4734,1945 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A212"/>
+  <dimension ref="A1:O212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.75" style="17" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.75" style="17" customWidth="1"/>
+    <col min="6" max="8" width="9.875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.875" style="13" customWidth="1"/>
+    <col min="11" max="11" width="9.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="F1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="J1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="11">
+        <f>AVERAGE(K4:K63)</f>
+        <v>3.5166666666666666</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="16"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="11">
+        <f>AVERAGE(M4:M15)</f>
+        <v>17.583333333333332</v>
+      </c>
+      <c r="F3" s="1">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1">
+        <v>300</v>
+      </c>
+      <c r="H3" s="1">
+        <v>600</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="11">
+        <f>AVERAGE(O4:O9)</f>
+        <v>35.166666666666664</v>
+      </c>
+      <c r="F4" s="1">
+        <v>120</v>
+      </c>
+      <c r="G4" s="1">
+        <v>600</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J4" s="5">
+        <v>60</v>
+      </c>
+      <c r="K4" s="6">
+        <v>2</v>
+      </c>
+      <c r="L4" s="5">
+        <v>300</v>
+      </c>
+      <c r="M4" s="6">
+        <v>17</v>
+      </c>
+      <c r="N4" s="5">
+        <v>600</v>
+      </c>
+      <c r="O4" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F5" s="1">
+        <v>180</v>
+      </c>
+      <c r="G5" s="1">
+        <v>900</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1800</v>
+      </c>
+      <c r="J5" s="5">
+        <v>120</v>
+      </c>
+      <c r="K5" s="6">
+        <v>6</v>
+      </c>
+      <c r="L5" s="5">
+        <v>600</v>
+      </c>
+      <c r="M5" s="6">
+        <v>23</v>
+      </c>
+      <c r="N5" s="5">
+        <v>1200</v>
+      </c>
+      <c r="O5" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F6" s="1">
+        <v>240</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1200</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2400</v>
+      </c>
+      <c r="J6" s="5">
+        <v>180</v>
+      </c>
+      <c r="K6" s="6">
+        <v>2</v>
+      </c>
+      <c r="L6" s="5">
+        <v>900</v>
+      </c>
+      <c r="M6" s="6">
+        <v>11</v>
+      </c>
+      <c r="N6" s="5">
+        <v>1800</v>
+      </c>
+      <c r="O6" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F7" s="1">
+        <v>300</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1500</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J7" s="5">
+        <v>240</v>
+      </c>
+      <c r="K7" s="6">
+        <v>4</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1200</v>
+      </c>
+      <c r="M7" s="6">
+        <v>11</v>
+      </c>
+      <c r="N7" s="5">
+        <v>2400</v>
+      </c>
+      <c r="O7" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="F8" s="1">
+        <v>360</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1800</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3600</v>
+      </c>
+      <c r="J8" s="5">
+        <v>300</v>
+      </c>
+      <c r="K8" s="6">
+        <v>3</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1500</v>
+      </c>
+      <c r="M8" s="6">
+        <v>15</v>
+      </c>
+      <c r="N8" s="5">
+        <v>3000</v>
+      </c>
+      <c r="O8" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="F9" s="1">
+        <v>420</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2100</v>
+      </c>
+      <c r="J9" s="5">
+        <v>360</v>
+      </c>
+      <c r="K9" s="6">
+        <v>7</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1800</v>
+      </c>
+      <c r="M9" s="6">
+        <v>15</v>
+      </c>
+      <c r="N9" s="5">
+        <v>3600</v>
+      </c>
+      <c r="O9" s="6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>171</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="F10" s="1">
+        <v>480</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2400</v>
+      </c>
+      <c r="J10" s="5">
+        <v>420</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>2100</v>
+      </c>
+      <c r="M10" s="6">
+        <v>25</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>172</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="F11" s="1">
+        <v>540</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2700</v>
+      </c>
+      <c r="J11" s="5">
+        <v>480</v>
+      </c>
+      <c r="K11" s="6">
+        <v>4</v>
+      </c>
+      <c r="L11" s="5">
+        <v>2400</v>
+      </c>
+      <c r="M11" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>190</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="F12" s="1">
+        <v>600</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J12" s="5">
+        <v>540</v>
+      </c>
+      <c r="K12" s="6">
+        <v>9</v>
+      </c>
+      <c r="L12" s="5">
+        <v>2700</v>
+      </c>
+      <c r="M12" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>191</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="F13" s="1">
+        <v>660</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3300</v>
+      </c>
+      <c r="J13" s="5">
+        <v>600</v>
+      </c>
+      <c r="K13" s="6">
+        <v>3</v>
+      </c>
+      <c r="L13" s="5">
+        <v>3000</v>
+      </c>
+      <c r="M13" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>211</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="F14" s="1">
+        <v>720</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3600</v>
+      </c>
+      <c r="J14" s="5">
+        <v>660</v>
+      </c>
+      <c r="K14" s="6">
+        <v>4</v>
+      </c>
+      <c r="L14" s="5">
+        <v>3300</v>
+      </c>
+      <c r="M14" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>212</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="F15" s="1">
+        <v>780</v>
+      </c>
+      <c r="J15" s="5">
+        <v>720</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <v>3600</v>
+      </c>
+      <c r="M15" s="6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>245</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="F16" s="1">
+        <v>840</v>
+      </c>
+      <c r="J16" s="5">
+        <v>780</v>
+      </c>
+      <c r="K16" s="6">
+        <v>5</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>260</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="F17" s="1">
+        <v>900</v>
+      </c>
+      <c r="J17" s="5">
+        <v>840</v>
+      </c>
+      <c r="K17" s="6">
+        <v>2</v>
+      </c>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>261</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="F18" s="1">
+        <v>960</v>
+      </c>
+      <c r="J18" s="5">
+        <v>900</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>306</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="F19" s="1">
+        <v>1020</v>
+      </c>
+      <c r="J19" s="5">
+        <v>960</v>
+      </c>
+      <c r="K19" s="6">
+        <v>0</v>
+      </c>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>307</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="F20" s="1">
+        <v>1080</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1020</v>
+      </c>
+      <c r="K20" s="6">
+        <v>6</v>
+      </c>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>308</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="F21" s="1">
+        <v>1140</v>
+      </c>
+      <c r="J21" s="5">
+        <v>1080</v>
+      </c>
+      <c r="K21" s="6">
+        <v>1</v>
+      </c>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>309</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="F22" s="1">
+        <v>1200</v>
+      </c>
+      <c r="J22" s="5">
+        <v>1140</v>
+      </c>
+      <c r="K22" s="6">
+        <v>1</v>
+      </c>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>310</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="F23" s="1">
+        <v>1260</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1200</v>
+      </c>
+      <c r="K23" s="6">
+        <v>3</v>
+      </c>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>311</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="F24" s="1">
+        <v>1320</v>
+      </c>
+      <c r="J24" s="5">
+        <v>1260</v>
+      </c>
+      <c r="K24" s="6">
+        <v>2</v>
+      </c>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>348</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="F25" s="1">
+        <v>1380</v>
+      </c>
+      <c r="J25" s="5">
+        <v>1320</v>
+      </c>
+      <c r="K25" s="6">
+        <v>4</v>
+      </c>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>428</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="F26" s="1">
+        <v>1440</v>
+      </c>
+      <c r="J26" s="5">
+        <v>1380</v>
+      </c>
+      <c r="K26" s="6">
+        <v>5</v>
+      </c>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>452</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="F27" s="1">
+        <v>1500</v>
+      </c>
+      <c r="J27" s="5">
+        <v>1440</v>
+      </c>
+      <c r="K27" s="6">
+        <v>1</v>
+      </c>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>453</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="F28" s="1">
+        <v>1560</v>
+      </c>
+      <c r="J28" s="5">
+        <v>1500</v>
+      </c>
+      <c r="K28" s="6">
+        <v>3</v>
+      </c>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>468</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="F29" s="1">
+        <v>1620</v>
+      </c>
+      <c r="J29" s="5">
+        <v>1560</v>
+      </c>
+      <c r="K29" s="6">
+        <v>2</v>
+      </c>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="F30" s="1">
+        <v>1680</v>
+      </c>
+      <c r="J30" s="5">
+        <v>1620</v>
+      </c>
+      <c r="K30" s="6">
+        <v>4</v>
+      </c>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>518</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="F31" s="1">
+        <v>1740</v>
+      </c>
+      <c r="J31" s="5">
+        <v>1680</v>
+      </c>
+      <c r="K31" s="6">
+        <v>3</v>
+      </c>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>519</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="F32" s="1">
+        <v>1800</v>
+      </c>
+      <c r="J32" s="5">
+        <v>1740</v>
+      </c>
+      <c r="K32" s="6">
+        <v>4</v>
+      </c>
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>520</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="F33" s="1">
+        <v>1860</v>
+      </c>
+      <c r="J33" s="5">
+        <v>1800</v>
+      </c>
+      <c r="K33" s="6">
+        <v>2</v>
+      </c>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>521</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="F34" s="1">
+        <v>1920</v>
+      </c>
+      <c r="J34" s="5">
+        <v>1860</v>
+      </c>
+      <c r="K34" s="6">
+        <v>5</v>
+      </c>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>522</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="F35" s="1">
+        <v>1980</v>
+      </c>
+      <c r="J35" s="5">
+        <v>1920</v>
+      </c>
+      <c r="K35" s="6">
+        <v>5</v>
+      </c>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>538</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="F36" s="1">
+        <v>2040</v>
+      </c>
+      <c r="J36" s="5">
+        <v>1980</v>
+      </c>
+      <c r="K36" s="6">
+        <v>3</v>
+      </c>
+      <c r="L36" s="6"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>539</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="F37" s="1">
+        <v>2100</v>
+      </c>
+      <c r="J37" s="5">
+        <v>2040</v>
+      </c>
+      <c r="K37" s="6">
+        <v>2</v>
+      </c>
+      <c r="L37" s="6"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>540</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="F38" s="1">
+        <v>2160</v>
+      </c>
+      <c r="J38" s="5">
+        <v>2100</v>
+      </c>
+      <c r="K38" s="6">
+        <v>10</v>
+      </c>
+      <c r="L38" s="6"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>541</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="F39" s="1">
+        <v>2220</v>
+      </c>
+      <c r="J39" s="5">
+        <v>2160</v>
+      </c>
+      <c r="K39" s="6">
+        <v>3</v>
+      </c>
+      <c r="L39" s="6"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>542</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="F40" s="1">
+        <v>2280</v>
+      </c>
+      <c r="J40" s="5">
+        <v>2220</v>
+      </c>
+      <c r="K40" s="6">
+        <v>3</v>
+      </c>
+      <c r="L40" s="6"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>543</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="F41" s="1">
+        <v>2340</v>
+      </c>
+      <c r="J41" s="5">
+        <v>2280</v>
+      </c>
+      <c r="K41" s="6">
+        <v>0</v>
+      </c>
+      <c r="L41" s="6"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>619</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="F42" s="1">
+        <v>2400</v>
+      </c>
+      <c r="J42" s="5">
+        <v>2340</v>
+      </c>
+      <c r="K42" s="6">
+        <v>5</v>
+      </c>
+      <c r="L42" s="6"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>620</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="F43" s="1">
+        <v>2460</v>
+      </c>
+      <c r="J43" s="5">
+        <v>2400</v>
+      </c>
+      <c r="K43" s="6">
+        <v>1</v>
+      </c>
+      <c r="L43" s="6"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>630</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="F44" s="1">
+        <v>2520</v>
+      </c>
+      <c r="J44" s="5">
+        <v>2460</v>
+      </c>
+      <c r="K44" s="6">
+        <v>2</v>
+      </c>
+      <c r="L44" s="6"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>658</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="F45" s="1">
+        <v>2580</v>
+      </c>
+      <c r="J45" s="5">
+        <v>2520</v>
+      </c>
+      <c r="K45" s="6">
+        <v>4</v>
+      </c>
+      <c r="L45" s="6"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>736</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="F46" s="1">
+        <v>2640</v>
+      </c>
+      <c r="J46" s="5">
+        <v>2580</v>
+      </c>
+      <c r="K46" s="6">
+        <v>2</v>
+      </c>
+      <c r="L46" s="6"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>766</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="F47" s="1">
+        <v>2700</v>
+      </c>
+      <c r="J47" s="5">
+        <v>2640</v>
+      </c>
+      <c r="K47" s="6">
+        <v>0</v>
+      </c>
+      <c r="L47" s="6"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>770</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="F48" s="1">
+        <v>2760</v>
+      </c>
+      <c r="J48" s="5">
+        <v>2700</v>
+      </c>
+      <c r="K48" s="6">
+        <v>2</v>
+      </c>
+      <c r="L48" s="6"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>771</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="F49" s="1">
+        <v>2820</v>
+      </c>
+      <c r="J49" s="5">
+        <v>2760</v>
+      </c>
+      <c r="K49" s="6">
+        <v>5</v>
+      </c>
+      <c r="L49" s="6"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>772</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="F50" s="1">
+        <v>2880</v>
+      </c>
+      <c r="J50" s="5">
+        <v>2820</v>
+      </c>
+      <c r="K50" s="6">
+        <v>2</v>
+      </c>
+      <c r="L50" s="6"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>815</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="F51" s="1">
+        <v>2940</v>
+      </c>
+      <c r="J51" s="5">
+        <v>2880</v>
+      </c>
+      <c r="K51" s="6">
+        <v>2</v>
+      </c>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>816</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="F52" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J52" s="5">
+        <v>2940</v>
+      </c>
+      <c r="K52" s="6">
+        <v>1</v>
+      </c>
+      <c r="L52" s="6"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>980</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="F53" s="1">
+        <v>3060</v>
+      </c>
+      <c r="J53" s="5">
+        <v>3000</v>
+      </c>
+      <c r="K53" s="6">
+        <v>8</v>
+      </c>
+      <c r="L53" s="6"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>994</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="F54" s="1">
+        <v>3120</v>
+      </c>
+      <c r="J54" s="5">
+        <v>3060</v>
+      </c>
+      <c r="K54" s="6">
+        <v>6</v>
+      </c>
+      <c r="L54" s="6"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>995</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="F55" s="1">
+        <v>3180</v>
+      </c>
+      <c r="J55" s="5">
+        <v>3120</v>
+      </c>
+      <c r="K55" s="6">
+        <v>1</v>
+      </c>
+      <c r="L55" s="6"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>996</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="F56" s="1">
+        <v>3240</v>
+      </c>
+      <c r="J56" s="5">
+        <v>3180</v>
+      </c>
+      <c r="K56" s="6">
+        <v>4</v>
+      </c>
+      <c r="L56" s="6"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>997</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="F57" s="1">
+        <v>3300</v>
+      </c>
+      <c r="J57" s="5">
+        <v>3240</v>
+      </c>
+      <c r="K57" s="6">
+        <v>10</v>
+      </c>
+      <c r="L57" s="6"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>1010</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="F58" s="1">
+        <v>3360</v>
+      </c>
+      <c r="J58" s="5">
+        <v>3300</v>
+      </c>
+      <c r="K58" s="6">
+        <v>4</v>
+      </c>
+      <c r="L58" s="6"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>1060</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="F59" s="1">
+        <v>3420</v>
+      </c>
+      <c r="J59" s="5">
+        <v>3360</v>
+      </c>
+      <c r="K59" s="6">
+        <v>9</v>
+      </c>
+      <c r="L59" s="6"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>1114</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="F60" s="1">
+        <v>3480</v>
+      </c>
+      <c r="J60" s="5">
+        <v>3420</v>
+      </c>
+      <c r="K60" s="6">
+        <v>3</v>
+      </c>
+      <c r="L60" s="6"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>1157</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="F61" s="1">
+        <v>3540</v>
+      </c>
+      <c r="J61" s="5">
+        <v>3480</v>
+      </c>
+      <c r="K61" s="6">
+        <v>3</v>
+      </c>
+      <c r="L61" s="6"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>1185</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="F62" s="1">
+        <v>3600</v>
+      </c>
+      <c r="J62" s="5">
+        <v>3540</v>
+      </c>
+      <c r="K62" s="6">
+        <v>6</v>
+      </c>
+      <c r="L62" s="6"/>
+    </row>
+    <row r="63" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
         <v>1186</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="J63" s="5">
+        <v>3600</v>
+      </c>
+      <c r="K63" s="6">
+        <v>8</v>
+      </c>
+      <c r="L63" s="7"/>
+    </row>
+    <row r="64" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
         <v>1259</v>
       </c>
+      <c r="J64" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K64" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>1260</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>1278</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>1279</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>1280</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>1317</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="A70" s="1">
         <v>1326</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="A71" s="1">
         <v>1327</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72">
+      <c r="A72" s="1">
         <v>1339</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73">
+      <c r="A73" s="1">
         <v>1340</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74">
+      <c r="A74" s="1">
         <v>1373</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75">
+      <c r="A75" s="1">
         <v>1388</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76">
+      <c r="A76" s="1">
         <v>1472</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77">
+      <c r="A77" s="1">
         <v>1473</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="A78" s="1">
         <v>1474</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79">
+      <c r="A79" s="1">
         <v>1512</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80">
+      <c r="A80" s="1">
         <v>1524</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81">
+      <c r="A81" s="1">
         <v>1574</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82">
+      <c r="A82" s="1">
         <v>1582</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83">
+      <c r="A83" s="1">
         <v>1584</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="A84" s="1">
         <v>1585</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85">
+      <c r="A85" s="1">
         <v>1658</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86">
+      <c r="A86" s="1">
         <v>1659</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87">
+      <c r="A87" s="1">
         <v>1660</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88">
+      <c r="A88" s="1">
         <v>1700</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="A89" s="1">
         <v>1711</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90">
+      <c r="A90" s="1">
         <v>1712</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91">
+      <c r="A91" s="1">
         <v>1726</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92">
+      <c r="A92" s="1">
         <v>1754</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93">
+      <c r="A93" s="1">
         <v>1795</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94">
+      <c r="A94" s="1">
         <v>1820</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95">
+      <c r="A95" s="1">
         <v>1830</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96">
+      <c r="A96" s="1">
         <v>1831</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97">
+      <c r="A97" s="1">
         <v>1840</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98">
+      <c r="A98" s="1">
         <v>1860</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99">
+      <c r="A99" s="1">
         <v>1894</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100">
+      <c r="A100" s="1">
         <v>1900</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101">
+      <c r="A101" s="1">
         <v>1904</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102">
+      <c r="A102" s="1">
         <v>1905</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103">
+      <c r="A103" s="1">
         <v>1911</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104">
+      <c r="A104" s="1">
         <v>1948</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105">
+      <c r="A105" s="1">
         <v>1949</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106">
+      <c r="A106" s="1">
         <v>1950</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107">
+      <c r="A107" s="1">
         <v>3036</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108">
+      <c r="A108" s="1">
         <v>2038</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109">
+      <c r="A109" s="1">
         <v>2039</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110">
+      <c r="A110" s="1">
         <v>2067</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111">
+      <c r="A111" s="1">
         <v>2068</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112">
+      <c r="A112" s="1">
         <v>2085</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113">
+      <c r="A113" s="1">
         <v>2086</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114">
+      <c r="A114" s="1">
         <v>2087</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115">
+      <c r="A115" s="1">
         <v>2088</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116">
+      <c r="A116" s="1">
         <v>2089</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117">
+      <c r="A117" s="1">
         <v>2090</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118">
+      <c r="A118" s="1">
         <v>2091</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119">
+      <c r="A119" s="1">
         <v>2090</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120">
+      <c r="A120" s="1">
         <v>2107</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121">
+      <c r="A121" s="1">
         <v>2109</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122">
+      <c r="A122" s="1">
         <v>2125</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123">
+      <c r="A123" s="1">
         <v>2203</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124">
+      <c r="A124" s="1">
         <v>2204</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125">
+      <c r="A125" s="1">
         <v>2205</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126">
+      <c r="A126" s="1">
         <v>2292</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127">
+      <c r="A127" s="1">
         <v>2311</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128">
+      <c r="A128" s="1">
         <v>2312</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129">
+      <c r="A129" s="1">
         <v>2338</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130">
+      <c r="A130" s="1">
         <v>2339</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131">
+      <c r="A131" s="1">
         <v>2378</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132">
+      <c r="A132" s="1">
         <v>2408</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133">
+      <c r="A133" s="1">
         <v>2413</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134">
+      <c r="A134" s="1">
         <v>2471</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135">
+      <c r="A135" s="1">
         <v>2488</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136">
+      <c r="A136" s="1">
         <v>2489</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137">
+      <c r="A137" s="1">
         <v>2510</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138">
+      <c r="A138" s="1">
         <v>2552</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139">
+      <c r="A139" s="1">
         <v>2578</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140">
+      <c r="A140" s="1">
         <v>2675</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141">
+      <c r="A141" s="1">
         <v>2698</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142">
+      <c r="A142" s="1">
         <v>2705</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143">
+      <c r="A143" s="1">
         <v>2706</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144">
+      <c r="A144" s="1">
         <v>2716</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145">
+      <c r="A145" s="1">
         <v>2717</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146">
+      <c r="A146" s="1">
         <v>2760</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147">
+      <c r="A147" s="1">
         <v>2761</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148">
+      <c r="A148" s="1">
         <v>2818</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149">
+      <c r="A149" s="1">
         <v>2866</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150">
+      <c r="A150" s="1">
         <v>2867</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151">
+      <c r="A151" s="1">
         <v>2910</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152">
+      <c r="A152" s="1">
         <v>2941</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153">
+      <c r="A153" s="1">
         <v>2948</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154">
+      <c r="A154" s="1">
         <v>2949</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155">
+      <c r="A155" s="1">
         <v>2952</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156">
+      <c r="A156" s="1">
         <v>2966</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157">
+      <c r="A157" s="1">
         <v>2967</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158">
+      <c r="A158" s="1">
         <v>2972</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159">
+      <c r="A159" s="1">
         <v>3000</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160">
+      <c r="A160" s="1">
         <v>3013</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161">
+      <c r="A161" s="1">
         <v>3014</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162">
+      <c r="A162" s="1">
         <v>3015</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163">
+      <c r="A163" s="1">
         <v>3032</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164">
+      <c r="A164" s="1">
         <v>3033</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165">
+      <c r="A165" s="1">
         <v>3087</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166">
+      <c r="A166" s="1">
         <v>3138</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167">
+      <c r="A167" s="1">
         <v>3139</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168">
+      <c r="A168" s="1">
         <v>3177</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169">
+      <c r="A169" s="1">
         <v>3179</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170">
+      <c r="A170" s="1">
         <v>3181</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171">
+      <c r="A171" s="1">
         <v>3182</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172">
+      <c r="A172" s="1">
         <v>3197</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173">
+      <c r="A173" s="1">
         <v>3198</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174">
+      <c r="A174" s="1">
         <v>3208</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175">
+      <c r="A175" s="1">
         <v>3209</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176">
+      <c r="A176" s="1">
         <v>3214</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177">
+      <c r="A177" s="1">
         <v>3215</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178">
+      <c r="A178" s="1">
         <v>3222</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179">
+      <c r="A179" s="1">
         <v>3233</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180">
+      <c r="A180" s="1">
         <v>3251</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181">
+      <c r="A181" s="1">
         <v>3252</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182">
+      <c r="A182" s="1">
         <v>3270</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183">
+      <c r="A183" s="1">
         <v>3311</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184">
+      <c r="A184" s="1">
         <v>3270</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185">
+      <c r="A185" s="1">
         <v>3311</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186">
+      <c r="A186" s="1">
         <v>3340</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187">
+      <c r="A187" s="1">
         <v>3342</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188">
+      <c r="A188" s="1">
         <v>3343</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189">
+      <c r="A189" s="1">
         <v>3352</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190">
+      <c r="A190" s="1">
         <v>3353</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191">
+      <c r="A191" s="1">
         <v>3358</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192">
+      <c r="A192" s="1">
         <v>3359</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193">
+      <c r="A193" s="1">
         <v>3361</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194">
+      <c r="A194" s="1">
         <v>3380</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195">
+      <c r="A195" s="1">
         <v>3420</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196">
+      <c r="A196" s="1">
         <v>3465</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197">
+      <c r="A197" s="1">
         <v>3466</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198">
+      <c r="A198" s="1">
         <v>3480</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199">
+      <c r="A199" s="1">
         <v>3483</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200">
+      <c r="A200" s="1">
         <v>3495</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201">
+      <c r="A201" s="1">
         <v>3510</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202">
+      <c r="A202" s="1">
         <v>3511</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203">
+      <c r="A203" s="1">
         <v>3515</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204">
+      <c r="A204" s="1">
         <v>3516</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205">
+      <c r="A205" s="1">
         <v>3550</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206">
+      <c r="A206" s="1">
         <v>3551</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207">
+      <c r="A207" s="1">
         <v>3552</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208">
+      <c r="A208" s="1">
         <v>3553</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209">
+      <c r="A209" s="1">
         <v>3556</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210">
+      <c r="A210" s="1">
         <v>3560</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211">
+      <c r="A211" s="1">
         <v>3561</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212">
+      <c r="A212" s="1">
         <v>3573</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="N4:N9">
+    <sortCondition ref="N4"/>
+  </sortState>
+  <mergeCells count="9">
+    <mergeCell ref="B1:B1048576"/>
+    <mergeCell ref="E1:E1048576"/>
+    <mergeCell ref="I1:I1048576"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4693,7 +6681,7 @@
   <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4788,10 +6776,10 @@
         <v>15.35</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>22</v>
@@ -4828,10 +6816,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="1">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1">
         <v>10</v>
-      </c>
-      <c r="J4" s="1">
-        <v>5</v>
       </c>
       <c r="L4" s="5">
         <v>10</v>
@@ -4868,10 +6856,10 @@
         <v>76</v>
       </c>
       <c r="I5" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J5" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L5" s="5">
         <v>20</v>
@@ -4897,10 +6885,10 @@
         <v>10</v>
       </c>
       <c r="I6" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="J6" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L6" s="5">
         <v>30</v>
@@ -4926,10 +6914,10 @@
         <v>9</v>
       </c>
       <c r="I7" s="1">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J7" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L7" s="5">
         <v>40</v>
@@ -4955,10 +6943,10 @@
         <v>15</v>
       </c>
       <c r="I8" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="J8" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L8" s="5">
         <v>50</v>
@@ -4984,10 +6972,10 @@
         <v>5</v>
       </c>
       <c r="I9" s="1">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="J9" s="1">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L9" s="5">
         <v>60</v>
@@ -5013,10 +7001,10 @@
         <v>19</v>
       </c>
       <c r="I10" s="1">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="J10" s="1">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="L10" s="5">
         <v>70</v>
@@ -5042,10 +7030,10 @@
         <v>13</v>
       </c>
       <c r="I11" s="1">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="J11" s="1">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="L11" s="5">
         <v>80</v>
@@ -5071,10 +7059,10 @@
         <v>55</v>
       </c>
       <c r="I12" s="1">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J12" s="1">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L12" s="5">
         <v>90</v>
@@ -5100,11 +7088,9 @@
         <v>5</v>
       </c>
       <c r="I13" s="1">
-        <v>100</v>
-      </c>
-      <c r="J13" s="1">
-        <v>50</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="J13" s="1"/>
       <c r="L13" s="5">
         <v>100</v>
       </c>
@@ -5129,7 +7115,7 @@
         <v>11</v>
       </c>
       <c r="I14" s="1">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J14" s="1"/>
       <c r="L14" s="5">
@@ -5156,7 +7142,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="1">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="J15" s="1"/>
       <c r="L15" s="5">
@@ -5179,7 +7165,7 @@
         <v>8</v>
       </c>
       <c r="I16" s="1">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="J16" s="1"/>
       <c r="L16" s="5">
@@ -5202,7 +7188,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="1">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="J17" s="1"/>
       <c r="L17" s="5">
@@ -5225,7 +7211,7 @@
         <v>5</v>
       </c>
       <c r="I18" s="1">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="J18" s="1"/>
       <c r="L18" s="5">
@@ -5248,7 +7234,7 @@
         <v>5</v>
       </c>
       <c r="I19" s="1">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="J19" s="1"/>
       <c r="L19" s="5">
@@ -5271,7 +7257,7 @@
         <v>8</v>
       </c>
       <c r="I20" s="1">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="J20" s="1"/>
       <c r="L20" s="5">
@@ -5292,7 +7278,7 @@
         <v>8</v>
       </c>
       <c r="I21" s="1">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="J21" s="1"/>
       <c r="L21" s="5">
@@ -5313,7 +7299,7 @@
         <v>15</v>
       </c>
       <c r="I22" s="1">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="J22" s="1"/>
       <c r="L22" s="5">
@@ -5334,7 +7320,7 @@
         <v>15</v>
       </c>
       <c r="I23" s="1">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="J23" s="1"/>
       <c r="L23" s="5">
@@ -5355,7 +7341,7 @@
         <v>3</v>
       </c>
       <c r="I24" s="1">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="J24" s="1"/>
       <c r="L24" s="5">
@@ -5376,7 +7362,7 @@
         <v>11</v>
       </c>
       <c r="I25" s="1">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="J25" s="1"/>
       <c r="L25" s="5">
@@ -5397,7 +7383,7 @@
         <v>10</v>
       </c>
       <c r="I26" s="1">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="J26" s="1"/>
       <c r="L26" s="5">
@@ -5418,7 +7404,7 @@
         <v>13</v>
       </c>
       <c r="I27" s="1">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="J27" s="1"/>
       <c r="L27" s="5">
@@ -5439,7 +7425,7 @@
         <v>11</v>
       </c>
       <c r="I28" s="1">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="J28" s="1"/>
       <c r="L28" s="5">
@@ -5460,7 +7446,7 @@
         <v>10</v>
       </c>
       <c r="I29" s="1">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="J29" s="1"/>
       <c r="L29" s="5">
@@ -5481,7 +7467,7 @@
         <v>6</v>
       </c>
       <c r="I30" s="1">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="J30" s="1"/>
       <c r="L30" s="5">
@@ -5502,7 +7488,7 @@
         <v>8</v>
       </c>
       <c r="I31" s="1">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="J31" s="1"/>
       <c r="L31" s="5">
@@ -5523,7 +7509,7 @@
         <v>9</v>
       </c>
       <c r="I32" s="1">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="J32" s="1"/>
       <c r="L32" s="5">
@@ -5543,10 +7529,6 @@
       <c r="C33" s="1">
         <v>22</v>
       </c>
-      <c r="I33" s="1">
-        <v>300</v>
-      </c>
-      <c r="J33" s="1"/>
       <c r="L33" s="5">
         <v>300</v>
       </c>

</xml_diff>